<commit_message>
updated bom, removed old one
</commit_message>
<xml_diff>
--- a/pcb/protopoint/protopoint_bom.xlsx
+++ b/pcb/protopoint/protopoint_bom.xlsx
@@ -15,45 +15,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Reference</t>
   </si>
   <si>
-    <t> Quantity</t>
-  </si>
-  <si>
-    <t> Value</t>
-  </si>
-  <si>
-    <t> Footprint</t>
-  </si>
-  <si>
-    <t> Datasheet</t>
-  </si>
-  <si>
-    <t> ManPartNo</t>
-  </si>
-  <si>
-    <t> DistPartNo</t>
-  </si>
-  <si>
-    <t>C1 C11 C3 </t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>ManPartNo</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>C34 </t>
+  </si>
+  <si>
+    <t>1.2pF</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_0201</t>
+  </si>
+  <si>
+    <t>GRM0335C1H1R2CA01D</t>
+  </si>
+  <si>
+    <t>490-6119-1-ND</t>
+  </si>
+  <si>
+    <t>C1, C3, C11 </t>
   </si>
   <si>
     <t>10pF</t>
   </si>
   <si>
-    <t>Capacitors_SMD:C_0201</t>
-  </si>
-  <si>
     <t>GRM0335C1E100JA01D</t>
   </si>
   <si>
     <t>490-8607-1-ND</t>
   </si>
   <si>
-    <t>C10 C17 C8 </t>
+    <t>C25, C26, C32, C36 </t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>GRM0335C1E120JA01D</t>
+  </si>
+  <si>
+    <t>490-3144-1-ND</t>
+  </si>
+  <si>
+    <t>C37, C38</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_0402</t>
+  </si>
+  <si>
+    <t>490-5924-1-ND</t>
+  </si>
+  <si>
+    <t>C35 </t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>GRM0335C1H180JA01D</t>
+  </si>
+  <si>
+    <t>490-6117-1-ND</t>
+  </si>
+  <si>
+    <t>C30 </t>
+  </si>
+  <si>
+    <t>27pF</t>
+  </si>
+  <si>
+    <t>GRM0335C1E270JA01D</t>
+  </si>
+  <si>
+    <t>490-3150-1-ND</t>
+  </si>
+  <si>
+    <t>C8, C10, C17</t>
   </si>
   <si>
     <t>100pF</t>
@@ -65,6 +119,30 @@
     <t>490-3160-1-ND</t>
   </si>
   <si>
+    <t>C5, C7 </t>
+  </si>
+  <si>
+    <t>330pF</t>
+  </si>
+  <si>
+    <t>GRM033R71E331KA01D</t>
+  </si>
+  <si>
+    <t>490-3178-1-ND</t>
+  </si>
+  <si>
+    <t>C31 </t>
+  </si>
+  <si>
+    <t>820pF</t>
+  </si>
+  <si>
+    <t>GRM033R71E821KA01D</t>
+  </si>
+  <si>
+    <t>490-3183-1-ND</t>
+  </si>
+  <si>
     <t>C12 </t>
   </si>
   <si>
@@ -77,7 +155,7 @@
     <t>490-3194-1-ND</t>
   </si>
   <si>
-    <t>C13 C14 C15 C16 C18 C19 C2 C20 C21 C23 C24 C27 C28 C29 C6 C9 </t>
+    <t>C2, C6, C9, C13, C14, C15, C16, C18, C19, C20, C21, C23, C24, C27, C28, C29</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -89,7 +167,7 @@
     <t>490-5881-1-ND</t>
   </si>
   <si>
-    <t>C22 C4 </t>
+    <t>C4, C22</t>
   </si>
   <si>
     <t>4.7uF</t>
@@ -104,42 +182,6 @@
     <t>490-3302-1-ND</t>
   </si>
   <si>
-    <t>C25 C26 C32 C36 </t>
-  </si>
-  <si>
-    <t>12pF</t>
-  </si>
-  <si>
-    <t>GRM0335C1E120JA01D</t>
-  </si>
-  <si>
-    <t>490-3144-1-ND</t>
-  </si>
-  <si>
-    <t>C30 </t>
-  </si>
-  <si>
-    <t>27pF</t>
-  </si>
-  <si>
-    <t>GRM0335C1E270JA01D</t>
-  </si>
-  <si>
-    <t>490-3150-1-ND</t>
-  </si>
-  <si>
-    <t>C31 </t>
-  </si>
-  <si>
-    <t>820pF</t>
-  </si>
-  <si>
-    <t>GRM033R71E821KA01D</t>
-  </si>
-  <si>
-    <t>490-3183-1-ND</t>
-  </si>
-  <si>
     <t>C33 </t>
   </si>
   <si>
@@ -152,57 +194,24 @@
     <t>490-7201-1-ND</t>
   </si>
   <si>
-    <t>C34 </t>
-  </si>
-  <si>
-    <t>1.2pF</t>
-  </si>
-  <si>
-    <t>GRM0335C1H1R2CA01D</t>
-  </si>
-  <si>
-    <t>490-6119-1-ND</t>
-  </si>
-  <si>
-    <t>C35 </t>
-  </si>
-  <si>
-    <t>18pF</t>
-  </si>
-  <si>
-    <t>GRM0335C1H180JA01D</t>
-  </si>
-  <si>
-    <t>490-6117-1-ND</t>
-  </si>
-  <si>
-    <t>C37 C38 </t>
-  </si>
-  <si>
-    <t>Capacitors_SMD:C_0402</t>
-  </si>
-  <si>
-    <t>C5 C7 </t>
-  </si>
-  <si>
-    <t>330pF</t>
-  </si>
-  <si>
-    <t>GRM033R71E331KA01D</t>
-  </si>
-  <si>
-    <t>490-3178-1-ND</t>
-  </si>
-  <si>
-    <t>R1 R2 R5 </t>
+    <t>R4 </t>
+  </si>
+  <si>
+    <t>Resistors_SMD:R_0201</t>
+  </si>
+  <si>
+    <t>ERJ-1GEF2700C</t>
+  </si>
+  <si>
+    <t>P270ABCT-ND</t>
+  </si>
+  <si>
+    <t>R1, R2, R5 </t>
   </si>
   <si>
     <t>11k</t>
   </si>
   <si>
-    <t>Resistors_SMD:R_0201</t>
-  </si>
-  <si>
     <t>ERJ-1GEF1102C</t>
   </si>
   <si>
@@ -221,9 +230,6 @@
     <t>P16.0KABCT-ND</t>
   </si>
   <si>
-    <t>R4 </t>
-  </si>
-  <si>
     <t>T1 </t>
   </si>
   <si>
@@ -293,16 +299,7 @@
     <t>863-1056-1-ND</t>
   </si>
   <si>
-    <t>U5 </t>
-  </si>
-  <si>
-    <t>ProtoPoint_Module</t>
-  </si>
-  <si>
-    <t>polypoint:ProtoPoint_Module_Castellated</t>
-  </si>
-  <si>
-    <t>X1 X2 </t>
+    <t>X1</t>
   </si>
   <si>
     <t>CRYSTAL_SMD_4</t>
@@ -315,6 +312,15 @@
   </si>
   <si>
     <t>SER3913CT-ND</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>FA-20H 38.4000MF10Z-AS3</t>
+  </si>
+  <si>
+    <t>SER3631CT-ND</t>
   </si>
 </sst>
 </file>
@@ -431,22 +437,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.4591836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.93877551020408"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8571428571429"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.9387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,248 +473,245 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,18 +719,18 @@
         <v>55</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="0" t="s">
         <v>58</v>
       </c>
     </row>
@@ -737,187 +739,199 @@
         <v>59</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>270</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>270</v>
-      </c>
       <c r="D17" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>76</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>97</v>
+      <c r="E24" s="0" t="s">
+        <v>100</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>